<commit_message>
update acs data and pod costs
</commit_message>
<xml_diff>
--- a/data/02-processed/pod_costs_budget.xlsx
+++ b/data/02-processed/pod_costs_budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenni\GHL\final-project-dabp\data\02-processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D2040E-31B6-4D4B-BDDB-68C9F04E710B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EF321F-7797-454A-897C-953EC444ABD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,8 +72,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="169" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -107,8 +107,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -482,22 +482,22 @@
         <v>24</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E9" si="0">B3*C3*D3</f>
+        <f t="shared" ref="E3:E5" si="0">B3*C3*D3</f>
         <v>12600</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F9" si="1">A3*2.25</f>
+        <f t="shared" ref="F3:F5" si="1">A3*2.25</f>
         <v>22500</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H9" si="2">F3*G3*1</f>
+        <f t="shared" ref="H3:H5" si="2">F3*G3*1</f>
         <v>22500</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I17" si="3">H3+E3</f>
+        <f t="shared" ref="I3:I9" si="3">H3+E3</f>
         <v>35100</v>
       </c>
     </row>
@@ -569,398 +569,134 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="B6" s="1">
         <v>35</v>
       </c>
       <c r="C6" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1">
         <v>24</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
-        <v>16800</v>
+        <f t="shared" ref="E6:E9" si="4">B6*C6*D6</f>
+        <v>12600</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="1"/>
-        <v>22500</v>
+        <f>A6*2.25</f>
+        <v>45000</v>
       </c>
       <c r="G6" s="3">
         <v>0.5</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="2"/>
-        <v>11250</v>
+        <f>F6*G6*1</f>
+        <v>22500</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" si="3"/>
-        <v>28050</v>
+        <v>35100</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="B7" s="1">
         <v>35</v>
       </c>
       <c r="C7" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1">
         <v>24</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>16800</v>
+        <f t="shared" si="4"/>
+        <v>12600</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="1"/>
-        <v>22500</v>
+        <f t="shared" ref="F7:F9" si="5">A7*2.25</f>
+        <v>45000</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" si="2"/>
-        <v>22500</v>
+        <f>F7*G7*1</f>
+        <v>45000</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="3"/>
-        <v>39300</v>
+        <v>57600</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="B8" s="1">
         <v>35</v>
       </c>
       <c r="C8" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1">
         <v>24</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>16800</v>
+        <f t="shared" si="4"/>
+        <v>12600</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="1"/>
-        <v>22500</v>
+        <f t="shared" si="5"/>
+        <v>45000</v>
       </c>
       <c r="G8" s="3">
         <v>3</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" si="2"/>
-        <v>67500</v>
+        <f t="shared" ref="H8:H9" si="6">F8*G8*1</f>
+        <v>135000</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="3"/>
-        <v>84300</v>
+        <v>147600</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="B9" s="1">
         <v>35</v>
       </c>
       <c r="C9" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1">
         <v>24</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="0"/>
-        <v>16800</v>
+        <f t="shared" si="4"/>
+        <v>12600</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="1"/>
-        <v>22500</v>
+        <f t="shared" si="5"/>
+        <v>45000</v>
       </c>
       <c r="G9" s="3">
         <v>5</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" si="2"/>
-        <v>112500</v>
+        <f t="shared" si="6"/>
+        <v>225000</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="3"/>
-        <v>129300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>20000</v>
-      </c>
-      <c r="B10" s="1">
-        <v>35</v>
-      </c>
-      <c r="C10" s="2">
-        <v>15</v>
-      </c>
-      <c r="D10" s="1">
-        <v>24</v>
-      </c>
-      <c r="E10" s="2">
-        <f>B10*C10*D10</f>
-        <v>12600</v>
-      </c>
-      <c r="F10" s="1">
-        <f>A10*2.25</f>
-        <v>45000</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H10" s="2">
-        <f>F10*G10*1</f>
-        <v>22500</v>
-      </c>
-      <c r="I10" s="2">
-        <f t="shared" si="3"/>
-        <v>35100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>20000</v>
-      </c>
-      <c r="B11" s="1">
-        <v>35</v>
-      </c>
-      <c r="C11" s="2">
-        <v>15</v>
-      </c>
-      <c r="D11" s="1">
-        <v>24</v>
-      </c>
-      <c r="E11" s="2">
-        <f>B11*C11*D11</f>
-        <v>12600</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" ref="F11:F16" si="4">A11*2.25</f>
-        <v>45000</v>
-      </c>
-      <c r="G11" s="3">
-        <v>1</v>
-      </c>
-      <c r="H11" s="2">
-        <f>F11*G11*1</f>
-        <v>45000</v>
-      </c>
-      <c r="I11" s="2">
-        <f t="shared" si="3"/>
-        <v>57600</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>20000</v>
-      </c>
-      <c r="B12" s="1">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2">
-        <v>15</v>
-      </c>
-      <c r="D12" s="1">
-        <v>24</v>
-      </c>
-      <c r="E12" s="2">
-        <f>B12*C12*D12</f>
-        <v>12600</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" si="4"/>
-        <v>45000</v>
-      </c>
-      <c r="G12" s="3">
-        <v>3</v>
-      </c>
-      <c r="H12" s="2">
-        <f t="shared" ref="H12:H17" si="5">F12*G12*1</f>
-        <v>135000</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="3"/>
-        <v>147600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>20000</v>
-      </c>
-      <c r="B13" s="1">
-        <v>35</v>
-      </c>
-      <c r="C13" s="2">
-        <v>15</v>
-      </c>
-      <c r="D13" s="1">
-        <v>24</v>
-      </c>
-      <c r="E13" s="2">
-        <f>B13*C13*D13</f>
-        <v>12600</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" si="4"/>
-        <v>45000</v>
-      </c>
-      <c r="G13" s="3">
-        <v>5</v>
-      </c>
-      <c r="H13" s="2">
-        <f t="shared" si="5"/>
-        <v>225000</v>
-      </c>
-      <c r="I13" s="2">
-        <f t="shared" si="3"/>
         <v>237600</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>20000</v>
-      </c>
-      <c r="B14" s="1">
-        <v>35</v>
-      </c>
-      <c r="C14" s="2">
-        <v>20</v>
-      </c>
-      <c r="D14" s="1">
-        <v>24</v>
-      </c>
-      <c r="E14" s="2">
-        <f>B14*C14*D14</f>
-        <v>16800</v>
-      </c>
-      <c r="F14" s="1">
-        <f t="shared" si="4"/>
-        <v>45000</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H14" s="2">
-        <f t="shared" si="5"/>
-        <v>22500</v>
-      </c>
-      <c r="I14" s="2">
-        <f t="shared" si="3"/>
-        <v>39300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>20000</v>
-      </c>
-      <c r="B15" s="1">
-        <v>35</v>
-      </c>
-      <c r="C15" s="2">
-        <v>20</v>
-      </c>
-      <c r="D15" s="1">
-        <v>24</v>
-      </c>
-      <c r="E15" s="2">
-        <f>B15*C15*D15</f>
-        <v>16800</v>
-      </c>
-      <c r="F15" s="1">
-        <f t="shared" si="4"/>
-        <v>45000</v>
-      </c>
-      <c r="G15" s="3">
-        <v>1</v>
-      </c>
-      <c r="H15" s="2">
-        <f t="shared" si="5"/>
-        <v>45000</v>
-      </c>
-      <c r="I15" s="2">
-        <f t="shared" si="3"/>
-        <v>61800</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
-        <v>20000</v>
-      </c>
-      <c r="B16" s="1">
-        <v>35</v>
-      </c>
-      <c r="C16" s="2">
-        <v>20</v>
-      </c>
-      <c r="D16" s="1">
-        <v>24</v>
-      </c>
-      <c r="E16" s="2">
-        <f>B16*C16*D16</f>
-        <v>16800</v>
-      </c>
-      <c r="F16" s="1">
-        <f t="shared" si="4"/>
-        <v>45000</v>
-      </c>
-      <c r="G16" s="3">
-        <v>3</v>
-      </c>
-      <c r="H16" s="2">
-        <f t="shared" si="5"/>
-        <v>135000</v>
-      </c>
-      <c r="I16" s="2">
-        <f t="shared" si="3"/>
-        <v>151800</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
-        <v>20000</v>
-      </c>
-      <c r="B17" s="1">
-        <v>35</v>
-      </c>
-      <c r="C17" s="2">
-        <v>20</v>
-      </c>
-      <c r="D17" s="1">
-        <v>24</v>
-      </c>
-      <c r="E17" s="2">
-        <f>B17*C17*D17</f>
-        <v>16800</v>
-      </c>
-      <c r="F17" s="1">
-        <f>A17*2.25</f>
-        <v>45000</v>
-      </c>
-      <c r="G17" s="3">
-        <v>5</v>
-      </c>
-      <c r="H17" s="2">
-        <f t="shared" si="5"/>
-        <v>225000</v>
-      </c>
-      <c r="I17" s="2">
-        <f t="shared" si="3"/>
-        <v>241800</v>
       </c>
     </row>
   </sheetData>
@@ -971,7 +707,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F385C10-BA3C-42DA-81EE-76D15AE628AF}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -987,52 +723,22 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>2000000</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>3000000</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>4000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>6000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>7000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
         <v>8000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>9000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>10000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>